<commit_message>
Added ArithUnit and Adder
-"do FunctionalLogicUnit.do" fails
</commit_message>
<xml_diff>
--- a/Exu/Documentation/FP1-log-G57-8414-350-1201.xlsx
+++ b/Exu/Documentation/FP1-log-G57-8414-350-1201.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Marco\Desktop\ENSC350FP\Exu\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C23AFE-9114-4E50-BAB6-43D8D60C086B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B012E43-C8E3-4E4B-A2CE-193E3ADAD644}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="-22050" yWindow="690" windowWidth="21600" windowHeight="11505" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>Set up Quartus Project</t>
+  </si>
+  <si>
+    <t>Write LogicUnit.vhd + Set up TBLogicUnit</t>
+  </si>
+  <si>
+    <t>Write Adder.vhd</t>
+  </si>
+  <si>
+    <t>Write ArithUnit.vhd</t>
   </si>
 </sst>
 </file>
@@ -667,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G756"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,7 +763,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
+      <c r="B7" s="13">
+        <v>8414</v>
+      </c>
       <c r="C7" s="9">
         <v>43917</v>
       </c>
@@ -769,7 +780,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
+      <c r="B8" s="13">
+        <v>8414</v>
+      </c>
       <c r="C8" s="9">
         <v>43917</v>
       </c>
@@ -784,25 +797,55 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="22"/>
-      <c r="G9" s="13"/>
+      <c r="B9" s="13">
+        <v>8414</v>
+      </c>
+      <c r="C9" s="10">
+        <v>43920</v>
+      </c>
+      <c r="D9" s="19">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E9" s="22">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="22"/>
-      <c r="G10" s="13"/>
+      <c r="B10" s="13">
+        <v>8414</v>
+      </c>
+      <c r="C10" s="10">
+        <v>43920</v>
+      </c>
+      <c r="D10" s="19">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="E10" s="22">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="13"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="22"/>
-      <c r="G11" s="13"/>
+      <c r="B11" s="13">
+        <v>8414</v>
+      </c>
+      <c r="C11" s="10">
+        <v>43920</v>
+      </c>
+      <c r="D11" s="19">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E11" s="22">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>

</xml_diff>

<commit_message>
Fixed Logic of AltB and AltBu in ArithUnit
</commit_message>
<xml_diff>
--- a/Exu/Documentation/FP1-log-G57-8414-350-1201.xlsx
+++ b/Exu/Documentation/FP1-log-G57-8414-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Marco\Desktop\ENSC350FP\Exu\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED5078F-5DAD-4A01-BBBF-9D5E7819845E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4157DF30-CC18-44F5-B631-F2721835F8F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22050" yWindow="690" windowWidth="21600" windowHeight="11505" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Set up Quartus Project</t>
   </si>
   <si>
-    <t>Write LogicUnit.vhd + Set up TBLogicUnit</t>
-  </si>
-  <si>
     <t>Write Adder.vhd</t>
   </si>
   <si>
@@ -96,6 +93,15 @@
   </si>
   <si>
     <t>Logic Unit Synthesis in Quartus</t>
+  </si>
+  <si>
+    <t>Logic Unit Timing Simulation and Timing Waves Screenshots</t>
+  </si>
+  <si>
+    <t>Write LogicUnit.vhd + Set up Testing Environment</t>
+  </si>
+  <si>
+    <t>Fixed Logic of AltB and AltBu</t>
   </si>
 </sst>
 </file>
@@ -682,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G756"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,7 +822,7 @@
         <v>0.73958333333333337</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -833,7 +839,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -850,7 +856,7 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -867,7 +873,7 @@
         <v>0.86458333333333337</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -884,27 +890,53 @@
         <v>0.875</v>
       </c>
       <c r="G13" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="13">
+        <v>8414</v>
+      </c>
+      <c r="C14" s="10">
+        <v>43920</v>
+      </c>
+      <c r="D14" s="22">
+        <v>0.875</v>
+      </c>
+      <c r="E14" s="22">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="22"/>
-      <c r="G14" s="13"/>
-    </row>
     <row r="15" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="13"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="22"/>
-      <c r="G15" s="13"/>
+      <c r="B15" s="13">
+        <v>8414</v>
+      </c>
+      <c r="C15" s="10">
+        <v>43920</v>
+      </c>
+      <c r="D15" s="19">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E15" s="22">
+        <v>0.9375</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="19"/>
+      <c r="B16" s="13">
+        <v>8414</v>
+      </c>
+      <c r="C16" s="10">
+        <v>43920</v>
+      </c>
+      <c r="D16" s="22">
+        <v>0.9375</v>
+      </c>
       <c r="E16" s="22"/>
       <c r="G16" s="13"/>
     </row>

</xml_diff>

<commit_message>
All Tasks for ArithUnit
Screenshot requiring attention is prefixed with [REDO] tag
</commit_message>
<xml_diff>
--- a/Exu/Documentation/FP1-log-G57-8414-350-1201.xlsx
+++ b/Exu/Documentation/FP1-log-G57-8414-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Marco\Desktop\ENSC350FP\Exu\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4157DF30-CC18-44F5-B631-F2721835F8F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB4D5B4-83D6-4699-9164-86E5DB4402BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22050" yWindow="690" windowWidth="21600" windowHeight="11505" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -689,7 +689,7 @@
   <dimension ref="A1:G756"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>